<commit_message>
Cambios en bilbiografia procesada. Se modificaron el formato de los autores a uno estandar
</commit_message>
<xml_diff>
--- a/data/procesados/bibliografia_programas_proce.xlsx
+++ b/data/procesados/bibliografia_programas_proce.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\data\procesados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A601F6D-7DC3-459C-AA48-4AB1FA137954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5996E0C0-3556-4E99-8F41-261E0A71504B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="118">
   <si>
     <t>Carrera</t>
   </si>
@@ -94,39 +94,21 @@
     <t xml:space="preserve"> Física universitaria. </t>
   </si>
   <si>
-    <t xml:space="preserve"> YOUNG, HUGH D.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Hacia los Vectores. Un curso preparatorio para Física universitaria </t>
   </si>
   <si>
-    <t xml:space="preserve"> Di Paolo, J</t>
-  </si>
-  <si>
     <t xml:space="preserve">Física para la ciencia y la tecnología. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Tippler, P.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Introducción a las mediciones de laboratorio. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Maiztegui, Gleiser.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Física. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Serway</t>
-  </si>
-  <si>
     <t xml:space="preserve">Física clásica y moderna </t>
   </si>
   <si>
-    <t xml:space="preserve"> Gettys, W. E.</t>
-  </si>
-  <si>
     <t>Introd. a la Física</t>
   </si>
   <si>
@@ -145,9 +127,6 @@
     <t xml:space="preserve">Matemáticas discreta y combinatoria. </t>
   </si>
   <si>
-    <t xml:space="preserve"> GRIMALDI, R. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Matemática Discreta y sus aplicaciones. </t>
   </si>
   <si>
@@ -160,9 +139,6 @@
     <t xml:space="preserve">Química. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Chang, R. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Química Bioinorgánica. </t>
   </si>
   <si>
@@ -172,72 +148,36 @@
     <t xml:space="preserve">Química Inorgánica básica. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Cotton, A </t>
-  </si>
-  <si>
     <t xml:space="preserve">Química General. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Whitten, K. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Principios de Química </t>
   </si>
   <si>
-    <t xml:space="preserve"> Atkins, P. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Química Orgánica </t>
   </si>
   <si>
     <t xml:space="preserve">Organic Chemistry A Brief Survey of Concepts and Applications </t>
   </si>
   <si>
-    <t xml:space="preserve"> Philip S. Bailey, Jr.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Química Orgánica y Biológica </t>
   </si>
   <si>
     <t xml:space="preserve">Fundamentos de química orgánica </t>
   </si>
   <si>
-    <t xml:space="preserve"> YURKANIS BRUICE PAULA. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Fundamentals of Organic Chemistry </t>
   </si>
   <si>
-    <t xml:space="preserve"> John McMurry</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wade L. G. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Morrison y Boyd </t>
-  </si>
-  <si>
     <t xml:space="preserve">Química Biológica </t>
   </si>
   <si>
-    <t xml:space="preserve"> BLANCO A.</t>
-  </si>
-  <si>
     <t xml:space="preserve">principios de bioquímica </t>
   </si>
   <si>
-    <t xml:space="preserve"> Lehninger</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bioquímica </t>
   </si>
   <si>
-    <t xml:space="preserve"> Stryer Lubert</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Carey Francis A. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Química General, Orgánica y Biológica </t>
   </si>
   <si>
@@ -250,24 +190,15 @@
     <t xml:space="preserve">Algebra Lineal </t>
   </si>
   <si>
-    <t xml:space="preserve"> GROSSMAN, Stanley</t>
-  </si>
-  <si>
     <t xml:space="preserve">Algoritmos y Estructuras de Datos </t>
   </si>
   <si>
     <t xml:space="preserve">Estructuras de datos y algoritmos </t>
   </si>
   <si>
-    <t xml:space="preserve"> Aho, A. V.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grokking Algorithms: An Illustrated Guide for Programmers and Other Curious People. </t>
   </si>
   <si>
-    <t xml:space="preserve">  Bhargava, A.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Introduction to algorithms </t>
   </si>
   <si>
@@ -277,9 +208,6 @@
     <t xml:space="preserve">Hands-On Blockchain for Python Developers: Gain blockchain programming skills to build decentralized applications using Python. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Kok, A. S. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Solución de problemas con algoritmos y estructuras de datos usando Python </t>
   </si>
   <si>
@@ -382,7 +310,70 @@
     <t>serway, raymond a.</t>
   </si>
   <si>
-    <t>Tipler, Paul A.</t>
+    <t>tipler, paul a.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> maiztegui, alberto p.</t>
+  </si>
+  <si>
+    <t>gettys, w. edward</t>
+  </si>
+  <si>
+    <t>young, hugh d.</t>
+  </si>
+  <si>
+    <t>Grimaldi, Ralph P.</t>
+  </si>
+  <si>
+    <t>chang, raymond</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cotton, f. albert</t>
+  </si>
+  <si>
+    <t>whitten, kenneth w.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> atkins, peter</t>
+  </si>
+  <si>
+    <t>bailey, philip s.</t>
+  </si>
+  <si>
+    <t>yurkanis bruice, paula</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mcmurry, john</t>
+  </si>
+  <si>
+    <t>wade, l. g.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> morrison, robert thornton</t>
+  </si>
+  <si>
+    <t>blanco, antonio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lehninger, albert l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> stryer, lubert</t>
+  </si>
+  <si>
+    <t>carey, francis a.</t>
+  </si>
+  <si>
+    <t>grossman s., stanley i</t>
+  </si>
+  <si>
+    <t>Aho, Alfred V.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bhargava, aditya y.</t>
+  </si>
+  <si>
+    <t>kok, arjuna sky</t>
   </si>
 </sst>
 </file>
@@ -438,12 +429,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="C81" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,10 +1024,10 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1048,10 +1038,10 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D21" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,10 +1052,10 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>120</v>
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1076,10 +1066,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,10 +1080,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,10 +1094,10 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1121,7 +1111,7 @@
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,10 +1122,10 @@
         <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,10 +1136,10 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,10 +1150,10 @@
         <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1174,10 +1164,10 @@
         <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,10 +1178,10 @@
         <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1199,13 +1189,13 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1213,7 +1203,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
@@ -1227,7 +1217,7 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s">
         <v>19</v>
@@ -1241,7 +1231,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
@@ -1255,13 +1245,13 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1269,13 +1259,13 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1283,13 +1273,13 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1297,13 +1287,13 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,13 +1301,13 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,13 +1315,13 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1339,13 +1329,13 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1353,13 +1343,13 @@
         <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1367,13 +1357,13 @@
         <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1381,13 +1371,13 @@
         <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C45" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1395,13 +1385,13 @@
         <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1409,13 +1399,13 @@
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1423,13 +1413,13 @@
         <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1437,13 +1427,13 @@
         <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D49" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1451,13 +1441,13 @@
         <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C50" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1465,13 +1455,13 @@
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D51" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1479,13 +1469,13 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C52" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1493,13 +1483,13 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D53" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1507,13 +1497,13 @@
         <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1521,13 +1511,13 @@
         <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C55" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1535,13 +1525,13 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D56" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1549,13 +1539,13 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C57" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D57" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,13 +1553,13 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C58" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D58" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1577,13 +1567,13 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C59" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1591,13 +1581,13 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D60" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1605,13 +1595,13 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D61" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1619,13 +1609,13 @@
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C62" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D62" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1633,13 +1623,13 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1647,13 +1637,13 @@
         <v>14</v>
       </c>
       <c r="B64" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C64" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D64" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1661,13 +1651,13 @@
         <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C65" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D65" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,13 +1665,13 @@
         <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D66" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1689,13 +1679,13 @@
         <v>14</v>
       </c>
       <c r="B67" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C67" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D67" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1703,13 +1693,13 @@
         <v>14</v>
       </c>
       <c r="B68" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C68" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D68" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1717,13 +1707,13 @@
         <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C69" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D69" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1731,13 +1721,13 @@
         <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C70" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D70" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1745,13 +1735,13 @@
         <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C71" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D71" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1759,13 +1749,13 @@
         <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C72" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D72" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1773,13 +1763,13 @@
         <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C73" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D73" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1787,13 +1777,13 @@
         <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C74" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D74" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1801,7 +1791,7 @@
         <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C75" t="s">
         <v>13</v>
@@ -1815,13 +1805,13 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C76" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D76" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1829,7 +1819,7 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C77" t="s">
         <v>13</v>
@@ -1843,13 +1833,13 @@
         <v>15</v>
       </c>
       <c r="B78" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C78" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D78" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1857,7 +1847,7 @@
         <v>15</v>
       </c>
       <c r="B79" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C79" t="s">
         <v>13</v>
@@ -1871,13 +1861,13 @@
         <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C80" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D80" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1885,13 +1875,13 @@
         <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C81" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="D81" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1899,13 +1889,13 @@
         <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C82" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D82" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1913,13 +1903,13 @@
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C83" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D83" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,13 +1917,13 @@
         <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C84" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D84" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1941,13 +1931,13 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C85" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D85" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,13 +1945,13 @@
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C86" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="D86" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,13 +1959,13 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C87" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D87" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1983,13 +1973,13 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C88" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="D88" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1997,13 +1987,13 @@
         <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C89" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D89" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2011,13 +2001,13 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C90" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="D90" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2025,13 +2015,13 @@
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C91" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D91" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2039,13 +2029,13 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C92" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="D92" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2053,13 +2043,13 @@
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D93" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2067,13 +2057,13 @@
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C94" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D94" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2081,13 +2071,13 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="C95" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="D95" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,13 +2085,13 @@
         <v>4</v>
       </c>
       <c r="B96" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="C96" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D96" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2109,16 +2099,17 @@
         <v>4</v>
       </c>
       <c r="B97" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="C97" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="D97" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Terminamos de limpiar bibliografia
</commit_message>
<xml_diff>
--- a/data/procesados/bibliografia_programas_proce.xlsx
+++ b/data/procesados/bibliografia_programas_proce.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\data\procesados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F4AE82-B62C-43CC-AD29-8CEFA50C2DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA134B3-A391-432C-BC9C-5324D36391F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="117">
   <si>
     <t>Carrera</t>
   </si>
@@ -172,42 +172,24 @@
     <t xml:space="preserve">Solución de problemas con algoritmos y estructuras de datos usando Python </t>
   </si>
   <si>
-    <t xml:space="preserve"> Miller, B</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aspectos Legales del Uso de la Información </t>
   </si>
   <si>
     <t xml:space="preserve">Tratado de Derecho Constitucional </t>
   </si>
   <si>
-    <t xml:space="preserve">  ROSATTI Horacio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Código Civil y Comercial de la Nación </t>
   </si>
   <si>
-    <t xml:space="preserve"> Ricardo Luis LORENZETTI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Derecho Procesal Administrativo </t>
   </si>
   <si>
-    <t xml:space="preserve"> HUTCHINSON Tomás</t>
-  </si>
-  <si>
     <t xml:space="preserve">Acerca de la reflexión humana. La necesidad de detenernos y partir de la ignorancia </t>
   </si>
   <si>
     <t xml:space="preserve"> Guillermo MAGI</t>
   </si>
   <si>
-    <t xml:space="preserve">Tratado de derecho administrativo y obras selectas </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GORDILLO Agustín</t>
-  </si>
-  <si>
     <t xml:space="preserve">Desregulación, Entre el Derecho y la Economía </t>
   </si>
   <si>
@@ -368,6 +350,27 @@
   </si>
   <si>
     <t>mendenhall, william</t>
+  </si>
+  <si>
+    <t>ROSATTI Horacio</t>
+  </si>
+  <si>
+    <t>Miller, B</t>
+  </si>
+  <si>
+    <t>STEWART, James</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lorenzetti, ricardo luis</t>
+  </si>
+  <si>
+    <t>tomás hutchinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agustín a. gordillo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tratado de derecho administrativo. 5  </t>
   </si>
 </sst>
 </file>
@@ -423,12 +426,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +747,7 @@
     <col min="17" max="17" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,7 +761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -773,7 +775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -787,7 +789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -801,7 +803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -809,13 +811,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -823,13 +825,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -837,13 +839,13 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -851,13 +853,13 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -865,13 +867,13 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -879,13 +881,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -899,7 +901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -913,7 +915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -927,7 +929,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -941,7 +943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -955,7 +957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -969,7 +971,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -983,7 +985,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -997,7 +999,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1011,7 +1013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1019,13 +1021,13 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1033,13 +1035,13 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1050,10 +1052,10 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1064,10 +1066,10 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1075,13 +1077,13 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1089,13 +1091,13 @@
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1103,13 +1105,13 @@
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1117,13 +1119,13 @@
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1134,10 +1136,10 @@
         <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1148,10 +1150,10 @@
         <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1159,13 +1161,13 @@
         <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1173,13 +1175,13 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1193,7 +1195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1207,7 +1209,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1221,7 +1223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1235,7 +1237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1246,10 +1248,10 @@
         <v>28</v>
       </c>
       <c r="D36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1263,77 +1265,77 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
       <c r="B38" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
       <c r="B39" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
       <c r="B40" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
       <c r="B41" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" t="s">
         <v>36</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
       <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -1344,10 +1346,10 @@
         <v>32</v>
       </c>
       <c r="D43" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1361,7 +1363,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -1372,10 +1374,10 @@
         <v>35</v>
       </c>
       <c r="D45" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1386,10 +1388,10 @@
         <v>36</v>
       </c>
       <c r="D46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -1400,10 +1402,10 @@
         <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -1414,10 +1416,10 @@
         <v>32</v>
       </c>
       <c r="D48" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -1431,7 +1433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -1442,10 +1444,10 @@
         <v>35</v>
       </c>
       <c r="D50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -1456,10 +1458,10 @@
         <v>36</v>
       </c>
       <c r="D51" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -1470,10 +1472,10 @@
         <v>37</v>
       </c>
       <c r="D52" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -1481,290 +1483,290 @@
         <v>38</v>
       </c>
       <c r="C53" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>39</v>
+      </c>
+      <c r="C61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" t="s">
         <v>104</v>
       </c>
-      <c r="D53" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="2" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
         <v>39</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B55" s="2" t="s">
+      <c r="C62" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
         <v>39</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" t="s">
         <v>43</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
       <c r="B64" t="s">
         <v>39</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" t="s">
         <v>40</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>12</v>
       </c>
       <c r="B65" t="s">
         <v>39</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
       <c r="B66" t="s">
         <v>39</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
       <c r="B67" t="s">
         <v>39</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" t="s">
         <v>38</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
       <c r="B68" t="s">
         <v>39</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" t="s">
         <v>38</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
       <c r="B69" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" t="s">
         <v>41</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
       <c r="B70" t="s">
         <v>39</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>103</v>
+      </c>
+      <c r="D70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>12</v>
       </c>
       <c r="B71" t="s">
         <v>39</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" t="s">
         <v>42</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>12</v>
       </c>
       <c r="B72" t="s">
         <v>39</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" t="s">
         <v>38</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>12</v>
       </c>
       <c r="B73" t="s">
         <v>39</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" t="s">
         <v>43</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>108</v>
+      <c r="D73" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1778,7 +1780,7 @@
         <v>45</v>
       </c>
       <c r="D74" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1789,10 +1791,10 @@
         <v>44</v>
       </c>
       <c r="C75" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D75" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1806,7 +1808,7 @@
         <v>45</v>
       </c>
       <c r="D76" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1817,10 +1819,10 @@
         <v>44</v>
       </c>
       <c r="C77" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D77" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1834,7 +1836,7 @@
         <v>45</v>
       </c>
       <c r="D78" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1845,10 +1847,10 @@
         <v>44</v>
       </c>
       <c r="C79" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D79" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1862,7 +1864,7 @@
         <v>47</v>
       </c>
       <c r="D80" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1873,10 +1875,10 @@
         <v>46</v>
       </c>
       <c r="C81" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D81" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,7 +1892,7 @@
         <v>48</v>
       </c>
       <c r="D82" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1901,10 +1903,10 @@
         <v>46</v>
       </c>
       <c r="C83" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D83" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,7 +1920,7 @@
         <v>49</v>
       </c>
       <c r="D84" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,13 +1928,13 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85" t="s">
         <v>51</v>
       </c>
-      <c r="C85" t="s">
-        <v>52</v>
-      </c>
       <c r="D85" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1940,13 +1942,13 @@
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C86" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D86" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1954,13 +1956,13 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C87" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D87" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1968,13 +1970,13 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C88" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D88" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1982,13 +1984,13 @@
         <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C89" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="D89" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1996,13 +1998,13 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C90" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D90" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2010,13 +2012,13 @@
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C91" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D91" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2024,13 +2026,13 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C92" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D92" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2038,13 +2040,13 @@
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C93" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D93" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2052,13 +2054,13 @@
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C94" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D94" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2066,13 +2068,13 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C95" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D95" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2080,13 +2082,13 @@
         <v>4</v>
       </c>
       <c r="B96" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C96" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D96" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2094,13 +2096,13 @@
         <v>4</v>
       </c>
       <c r="B97" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C97" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D97" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Libros disponibles en biblioteca
</commit_message>
<xml_diff>
--- a/data/procesados/bibliografia_programas_proce.xlsx
+++ b/data/procesados/bibliografia_programas_proce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\data\procesados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA134B3-A391-432C-BC9C-5324D36391F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F676E7-6127-4519-94D8-8A662B1CC544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="118">
   <si>
     <t>Carrera</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tratado de derecho administrativo. 5  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cálculo de una Variable </t>
   </si>
 </sst>
 </file>
@@ -735,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +800,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Agregamos asignatura Espacio Integrador I al analisis
</commit_message>
<xml_diff>
--- a/data/procesados/bibliografia_programas_proce.xlsx
+++ b/data/procesados/bibliografia_programas_proce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\data\procesados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F676E7-6127-4519-94D8-8A662B1CC544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12805BA4-7652-41ED-9DDA-AA3D3062CD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="133">
   <si>
     <t>Carrera</t>
   </si>
@@ -374,6 +374,51 @@
   </si>
   <si>
     <t xml:space="preserve">Cálculo de una Variable </t>
+  </si>
+  <si>
+    <t>Espacio Integrador I</t>
+  </si>
+  <si>
+    <t>La investigación cualitativa y el análisis computarizado de datos</t>
+  </si>
+  <si>
+    <t>Echevarría, Hugo Darío</t>
+  </si>
+  <si>
+    <t>Scheaffer, Richard L</t>
+  </si>
+  <si>
+    <t>elementos de muestreo</t>
+  </si>
+  <si>
+    <t>tratamiento matemático de datos físico-químicos</t>
+  </si>
+  <si>
+    <t>Spiridinov, V.P.</t>
+  </si>
+  <si>
+    <t>computadoras y procesamiento de datos</t>
+  </si>
+  <si>
+    <t>Villanueva-Lara, Julio E</t>
+  </si>
+  <si>
+    <t>Introducción a la programación y a las estructuras de datos</t>
+  </si>
+  <si>
+    <t>Braunstein, Silvia L</t>
+  </si>
+  <si>
+    <t>Sheldom M. Ross</t>
+  </si>
+  <si>
+    <t>introducción a la estadística</t>
+  </si>
+  <si>
+    <t>Procesamiento de datos y análisis estadísticos</t>
+  </si>
+  <si>
+    <t>Castañeda, Ma. Belén</t>
   </si>
 </sst>
 </file>
@@ -736,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C91" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,6 +2153,104 @@
         <v>71</v>
       </c>
     </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98" t="s">
+        <v>118</v>
+      </c>
+      <c r="C98" t="s">
+        <v>119</v>
+      </c>
+      <c r="D98" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>4</v>
+      </c>
+      <c r="B99" t="s">
+        <v>118</v>
+      </c>
+      <c r="C99" t="s">
+        <v>122</v>
+      </c>
+      <c r="D99" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" t="s">
+        <v>118</v>
+      </c>
+      <c r="C100" t="s">
+        <v>123</v>
+      </c>
+      <c r="D100" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" t="s">
+        <v>118</v>
+      </c>
+      <c r="C101" t="s">
+        <v>125</v>
+      </c>
+      <c r="D101" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" t="s">
+        <v>118</v>
+      </c>
+      <c r="C102" t="s">
+        <v>127</v>
+      </c>
+      <c r="D102" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" t="s">
+        <v>118</v>
+      </c>
+      <c r="C103" t="s">
+        <v>130</v>
+      </c>
+      <c r="D103" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104" t="s">
+        <v>118</v>
+      </c>
+      <c r="C104" t="s">
+        <v>131</v>
+      </c>
+      <c r="D104" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambios en comparacion por asignatura ademas de normalizar datos en titulos y autores
</commit_message>
<xml_diff>
--- a/data/procesados/bibliografia_programas_proce.xlsx
+++ b/data/procesados/bibliografia_programas_proce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\data\procesados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12805BA4-7652-41ED-9DDA-AA3D3062CD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305F7876-86D9-44E3-96D7-C5463B8F3933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,12 +40,6 @@
     <t>Algebra y Cálculo</t>
   </si>
   <si>
-    <t xml:space="preserve">Álgebra lineal </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Grossman </t>
-  </si>
-  <si>
     <t xml:space="preserve">PRECÁLCULO </t>
   </si>
   <si>
@@ -419,6 +413,12 @@
   </si>
   <si>
     <t>Castañeda, Ma. Belén</t>
+  </si>
+  <si>
+    <t>grossman, stanley i.</t>
+  </si>
+  <si>
+    <t>Algebra lineal.</t>
   </si>
 </sst>
 </file>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C91" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,10 +817,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -831,10 +831,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -845,402 +845,402 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
         <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
         <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
         <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
         <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
         <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
         <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
         <v>94</v>
-      </c>
-      <c r="D21" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
-        <v>22</v>
-      </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
         <v>23</v>
-      </c>
-      <c r="C32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1248,13 +1248,13 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1262,13 +1262,13 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1276,629 +1276,629 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
         <v>27</v>
       </c>
-      <c r="C37" t="s">
-        <v>29</v>
-      </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
         <v>31</v>
       </c>
-      <c r="C39" t="s">
-        <v>33</v>
-      </c>
       <c r="D39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
         <v>31</v>
       </c>
-      <c r="C44" t="s">
-        <v>33</v>
-      </c>
       <c r="D44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D46" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D48" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" t="s">
         <v>31</v>
       </c>
-      <c r="C49" t="s">
-        <v>33</v>
-      </c>
       <c r="D49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D52" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C53" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D53" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D54" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D55" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C56" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" t="s">
         <v>98</v>
-      </c>
-      <c r="D56" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C57" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D57" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D58" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" t="s">
         <v>39</v>
       </c>
-      <c r="C59" t="s">
-        <v>41</v>
-      </c>
       <c r="D59" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C61" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D61" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C63" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D63" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D64" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C65" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D65" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C66" t="s">
+        <v>96</v>
+      </c>
+      <c r="D66" t="s">
         <v>98</v>
-      </c>
-      <c r="D66" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C67" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D67" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C68" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D68" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" t="s">
         <v>39</v>
       </c>
-      <c r="C69" t="s">
-        <v>41</v>
-      </c>
       <c r="D69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C70" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D70" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C71" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D71" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C72" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C73" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D73" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C74" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D74" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C75" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D75" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C76" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D76" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C77" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D77" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C78" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D78" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C79" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D79" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,13 +1906,13 @@
         <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C80" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D80" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,13 +1920,13 @@
         <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D81" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,13 +1934,13 @@
         <v>4</v>
       </c>
       <c r="B82" t="s">
+        <v>44</v>
+      </c>
+      <c r="C82" t="s">
         <v>46</v>
       </c>
-      <c r="C82" t="s">
-        <v>48</v>
-      </c>
       <c r="D82" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1948,13 +1948,13 @@
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C83" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D83" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1962,13 +1962,13 @@
         <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C84" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D84" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,13 +1976,13 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C85" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D85" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,13 +1990,13 @@
         <v>4</v>
       </c>
       <c r="B86" t="s">
+        <v>48</v>
+      </c>
+      <c r="C86" t="s">
         <v>50</v>
       </c>
-      <c r="C86" t="s">
-        <v>52</v>
-      </c>
       <c r="D86" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2004,13 +2004,13 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C87" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D87" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2018,13 +2018,13 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C88" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D88" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2032,13 +2032,13 @@
         <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C89" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D89" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2046,13 +2046,13 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C90" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D90" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,13 +2060,13 @@
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C91" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D91" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,13 +2074,13 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C92" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D92" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2088,13 +2088,13 @@
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C93" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D93" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,13 +2102,13 @@
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C94" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D94" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,13 +2116,13 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C95" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D95" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2130,13 +2130,13 @@
         <v>4</v>
       </c>
       <c r="B96" t="s">
+        <v>64</v>
+      </c>
+      <c r="C96" t="s">
         <v>66</v>
       </c>
-      <c r="C96" t="s">
-        <v>68</v>
-      </c>
       <c r="D96" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2144,13 +2144,13 @@
         <v>4</v>
       </c>
       <c r="B97" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C97" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D97" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,13 +2158,13 @@
         <v>4</v>
       </c>
       <c r="B98" t="s">
+        <v>116</v>
+      </c>
+      <c r="C98" t="s">
+        <v>117</v>
+      </c>
+      <c r="D98" t="s">
         <v>118</v>
-      </c>
-      <c r="C98" t="s">
-        <v>119</v>
-      </c>
-      <c r="D98" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2172,13 +2172,13 @@
         <v>4</v>
       </c>
       <c r="B99" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C99" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D99" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,13 +2186,13 @@
         <v>4</v>
       </c>
       <c r="B100" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C100" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D100" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,13 +2200,13 @@
         <v>4</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C101" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D101" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2214,13 +2214,13 @@
         <v>4</v>
       </c>
       <c r="B102" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C102" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D102" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2228,13 +2228,13 @@
         <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C103" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D103" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2242,13 +2242,13 @@
         <v>4</v>
       </c>
       <c r="B104" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C104" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D104" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Procesamos los titulos y autores de los programas
</commit_message>
<xml_diff>
--- a/data/procesados/bibliografia_programas_proce.xlsx
+++ b/data/procesados/bibliografia_programas_proce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\data\procesados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305F7876-86D9-44E3-96D7-C5463B8F3933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44686AAF-4D12-48DE-A8AE-E3DB4952034A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="124">
   <si>
     <t>Carrera</t>
   </si>
@@ -40,18 +40,27 @@
     <t>Algebra y Cálculo</t>
   </si>
   <si>
-    <t xml:space="preserve">PRECÁLCULO </t>
+    <t>algebra lineal</t>
+  </si>
+  <si>
+    <t>grossman, stanley i</t>
+  </si>
+  <si>
+    <t>precálculo</t>
+  </si>
+  <si>
+    <t>stewart, james</t>
+  </si>
+  <si>
+    <t>cálculo de una variable</t>
+  </si>
+  <si>
+    <t>Licenciatura en Bioinformática</t>
   </si>
   <si>
     <t xml:space="preserve">Cálculo en una Variable </t>
   </si>
   <si>
-    <t>Licenciatura en Bioinformática</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> STEWART, James</t>
-  </si>
-  <si>
     <t>Bioingeniería</t>
   </si>
   <si>
@@ -61,37 +70,58 @@
     <t xml:space="preserve">Fundamentos de Programación </t>
   </si>
   <si>
-    <t xml:space="preserve">El tutorial de Python. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Python Software Foundation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La Biblioteca Estándar de Python. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Python Software Foundation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referencia del Lenguaje Python. </t>
+    <t>el tutorial de python</t>
+  </si>
+  <si>
+    <t>python software foundation</t>
+  </si>
+  <si>
+    <t>la biblioteca estándar de python</t>
+  </si>
+  <si>
+    <t>referencia del lenguaje python</t>
   </si>
   <si>
     <t xml:space="preserve">Física Mecánica </t>
   </si>
   <si>
-    <t xml:space="preserve">Física para la ciencia y la tecnología. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introducción a las mediciones de laboratorio. </t>
+    <t>sears y zemansky física universitaria</t>
+  </si>
+  <si>
+    <t>young, hugh d</t>
+  </si>
+  <si>
+    <t>hacia los vectores</t>
+  </si>
+  <si>
+    <t>di paolo, josé</t>
+  </si>
+  <si>
+    <t>física para la ciencia y la tecnología</t>
+  </si>
+  <si>
+    <t>tipler, paul a</t>
+  </si>
+  <si>
+    <t>introducción a las mediciones de laboratorio</t>
+  </si>
+  <si>
+    <t>maiztegui, alberto p</t>
+  </si>
+  <si>
+    <t>física</t>
+  </si>
+  <si>
+    <t>serway, raymond a</t>
+  </si>
+  <si>
+    <t>gettys, w. edward</t>
   </si>
   <si>
     <t>Introd. a la Física</t>
   </si>
   <si>
-    <t xml:space="preserve">Física </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wilson, J. D.</t>
+    <t>wilson, j. d</t>
   </si>
   <si>
     <t xml:space="preserve">lnformática Básica </t>
@@ -100,325 +130,268 @@
     <t>Matemática Discreta</t>
   </si>
   <si>
-    <t xml:space="preserve">Matemáticas discreta y combinatoria. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matemática Discreta y sus aplicaciones. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ROSEN, Kenneth H</t>
+    <t>matemáticas discreta y combinatoria</t>
+  </si>
+  <si>
+    <t>grimaldi, ralph p</t>
+  </si>
+  <si>
+    <t>matemática discreta y sus aplicaciones</t>
+  </si>
+  <si>
+    <t>rosen, kenneth h</t>
   </si>
   <si>
     <t xml:space="preserve">Química General e Inorgánica </t>
   </si>
   <si>
-    <t xml:space="preserve">Química. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Química Bioinorgánica. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Baran Enrique J.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Química Inorgánica básica. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Química General. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Principios de Química </t>
+    <t>química</t>
+  </si>
+  <si>
+    <t>chang, raymond</t>
+  </si>
+  <si>
+    <t>química bioinorgánica</t>
+  </si>
+  <si>
+    <t>baran enrique j</t>
+  </si>
+  <si>
+    <t>química inorgánica básica</t>
+  </si>
+  <si>
+    <t>cotton, f. albert</t>
+  </si>
+  <si>
+    <t>química general</t>
+  </si>
+  <si>
+    <t>whitten, kenneth w</t>
+  </si>
+  <si>
+    <t>principios de química</t>
+  </si>
+  <si>
+    <t>atkins, peter</t>
   </si>
   <si>
     <t xml:space="preserve">Química Orgánica </t>
   </si>
   <si>
+    <t>química orgánica</t>
+  </si>
+  <si>
+    <t>bailey, philip s</t>
+  </si>
+  <si>
     <t xml:space="preserve">Química Orgánica y Biológica </t>
   </si>
   <si>
-    <t xml:space="preserve">Fundamentos de química orgánica </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Química Biológica </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bioquímica </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Química General, Orgánica y Biológica </t>
+    <t>fundamentos de química orgánica</t>
+  </si>
+  <si>
+    <t>yurkanis bruice, paula</t>
+  </si>
+  <si>
+    <t>mcmurry, john</t>
+  </si>
+  <si>
+    <t>wade, l. g</t>
+  </si>
+  <si>
+    <t>morrison, robert thornton</t>
+  </si>
+  <si>
+    <t>química biológica</t>
+  </si>
+  <si>
+    <t>blanco, antonio</t>
+  </si>
+  <si>
+    <t>bioquímica</t>
+  </si>
+  <si>
+    <t>lehninger, albert l</t>
+  </si>
+  <si>
+    <t>stryer, lubert</t>
+  </si>
+  <si>
+    <t>carey, francis a</t>
+  </si>
+  <si>
+    <t>química general, orgánica y biológica</t>
+  </si>
+  <si>
+    <t>wolfe drew h</t>
   </si>
   <si>
     <t xml:space="preserve">Álgebra Lineal y Geometría Analítica </t>
   </si>
   <si>
-    <t xml:space="preserve">Algebra Lineal </t>
+    <t>grossman s., stanley i</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmos y Estructuras de Datos </t>
   </si>
   <si>
-    <t xml:space="preserve">Estructuras de datos y algoritmos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to algorithms </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solución de problemas con algoritmos y estructuras de datos usando Python </t>
+    <t>estructuras de datos y algoritmos</t>
+  </si>
+  <si>
+    <t>aho, alfred v</t>
+  </si>
+  <si>
+    <t>grokking algorithms</t>
+  </si>
+  <si>
+    <t>bhargava, aditya y</t>
+  </si>
+  <si>
+    <t>introduction to algorithms</t>
+  </si>
+  <si>
+    <t>cormen, t. h</t>
+  </si>
+  <si>
+    <t>hands-on blockchain for python developers</t>
+  </si>
+  <si>
+    <t>kok, arjuna sky</t>
+  </si>
+  <si>
+    <t>solución de problemas con algoritmos y estructuras de datos usando python</t>
+  </si>
+  <si>
+    <t>miller, b</t>
   </si>
   <si>
     <t xml:space="preserve">Aspectos Legales del Uso de la Información </t>
   </si>
   <si>
-    <t xml:space="preserve">Tratado de Derecho Constitucional </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código Civil y Comercial de la Nación </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derecho Procesal Administrativo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acerca de la reflexión humana. La necesidad de detenernos y partir de la ignorancia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Guillermo MAGI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desregulación, Entre el Derecho y la Economía </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jorge Eduardo BUSTAMANTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sistema económico y rentístico </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ALBERDI, Juan B.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manual De Derecho Procesal Civil </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lino E. Palacio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contratos administrativos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SILVA CENSIO, Jorge A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nuevos Principios de Comercio Internacional, Para actuar en Escenarios Globalizados </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LEDESMA Carlos A</t>
+    <t>tratado de derecho constitucional</t>
+  </si>
+  <si>
+    <t>rosatti horacio</t>
+  </si>
+  <si>
+    <t>código civil y comercial de la nación</t>
+  </si>
+  <si>
+    <t>lorenzetti, ricardo luis</t>
+  </si>
+  <si>
+    <t>derecho procesal administrativo</t>
+  </si>
+  <si>
+    <t>tomás hutchinson</t>
+  </si>
+  <si>
+    <t>acerca de la reflexión humana. la necesidad de detenernos y partir de la ignorancia</t>
+  </si>
+  <si>
+    <t>guillermo magi</t>
+  </si>
+  <si>
+    <t>agustín a. gordillo</t>
+  </si>
+  <si>
+    <t>desregulación, entre el derecho y la economía</t>
+  </si>
+  <si>
+    <t>jorge eduardo bustamante</t>
+  </si>
+  <si>
+    <t>sistema económico y rentístico</t>
+  </si>
+  <si>
+    <t>alberdi, juan b</t>
+  </si>
+  <si>
+    <t>manual de derecho procesal civil</t>
+  </si>
+  <si>
+    <t>lino e. palacio</t>
+  </si>
+  <si>
+    <t>contratos administrativos</t>
+  </si>
+  <si>
+    <t>silva censio, jorge a</t>
+  </si>
+  <si>
+    <t>nuevos principios de comercio internacional, para actuar en escenarios globalizados</t>
+  </si>
+  <si>
+    <t>ledesma carlos a</t>
   </si>
   <si>
     <t xml:space="preserve">Probabilidad y Estadística </t>
   </si>
   <si>
-    <t xml:space="preserve">Introducción a la probabilidad y estadística. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estadística para todos. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RAMOS, EVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Probabilidad y estadística: enfoque por competencias. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GUTIERREZ BANEGAS, A. L.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> di paolo, josé</t>
-  </si>
-  <si>
-    <t>serway, raymond a.</t>
-  </si>
-  <si>
-    <t>tipler, paul a.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> maiztegui, alberto p.</t>
-  </si>
-  <si>
-    <t>gettys, w. edward</t>
-  </si>
-  <si>
-    <t>young, hugh d.</t>
-  </si>
-  <si>
-    <t>Grimaldi, Ralph P.</t>
-  </si>
-  <si>
-    <t>chang, raymond</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cotton, f. albert</t>
-  </si>
-  <si>
-    <t>whitten, kenneth w.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> atkins, peter</t>
-  </si>
-  <si>
-    <t>bailey, philip s.</t>
-  </si>
-  <si>
-    <t>yurkanis bruice, paula</t>
-  </si>
-  <si>
-    <t>wade, l. g.</t>
-  </si>
-  <si>
-    <t>blanco, antonio</t>
-  </si>
-  <si>
-    <t>carey, francis a.</t>
-  </si>
-  <si>
-    <t>grossman s., stanley i</t>
-  </si>
-  <si>
-    <t>Aho, Alfred V.</t>
-  </si>
-  <si>
-    <t>kok, arjuna sky</t>
-  </si>
-  <si>
-    <t>Cálculo de una variable</t>
-  </si>
-  <si>
-    <t>Precálculo</t>
-  </si>
-  <si>
-    <t>Sears y Zemansky Física universitaria</t>
-  </si>
-  <si>
-    <t>Hacia los Vectores</t>
-  </si>
-  <si>
-    <t>maiztegui, alberto p.</t>
-  </si>
-  <si>
-    <t>di paolo, josé</t>
-  </si>
-  <si>
-    <t>Física</t>
-  </si>
-  <si>
-    <t>Química orgánica</t>
-  </si>
-  <si>
-    <t>morrison, robert thornton</t>
-  </si>
-  <si>
-    <t>mcmurry, john</t>
-  </si>
-  <si>
-    <t>lehninger, albert l.</t>
-  </si>
-  <si>
-    <t>Wolfe Drew H.</t>
-  </si>
-  <si>
-    <t>Bioquímica</t>
-  </si>
-  <si>
-    <t>stryer, lubert</t>
-  </si>
-  <si>
-    <t>bhargava, aditya y.</t>
-  </si>
-  <si>
-    <t>Grokking Algorithms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cormen, T. H. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hands-On Blockchain for Python Developers </t>
+    <t>introducción a la probabilidad y estadística</t>
   </si>
   <si>
     <t>mendenhall, william</t>
   </si>
   <si>
-    <t>ROSATTI Horacio</t>
-  </si>
-  <si>
-    <t>Miller, B</t>
-  </si>
-  <si>
-    <t>STEWART, James</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lorenzetti, ricardo luis</t>
-  </si>
-  <si>
-    <t>tomás hutchinson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">agustín a. gordillo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratado de derecho administrativo. 5  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cálculo de una Variable </t>
+    <t>estadística para todos</t>
+  </si>
+  <si>
+    <t>ramos, eva</t>
+  </si>
+  <si>
+    <t>probabilidad y estadística: enfoque por competencias</t>
+  </si>
+  <si>
+    <t>gutierrez banegas, a. l</t>
   </si>
   <si>
     <t>Espacio Integrador I</t>
   </si>
   <si>
-    <t>La investigación cualitativa y el análisis computarizado de datos</t>
-  </si>
-  <si>
-    <t>Echevarría, Hugo Darío</t>
-  </si>
-  <si>
-    <t>Scheaffer, Richard L</t>
+    <t>la investigación cualitativa y el análisis computarizado de datos</t>
+  </si>
+  <si>
+    <t>echevarría, hugo darío</t>
   </si>
   <si>
     <t>elementos de muestreo</t>
   </si>
   <si>
+    <t>scheaffer, richard l</t>
+  </si>
+  <si>
     <t>tratamiento matemático de datos físico-químicos</t>
   </si>
   <si>
-    <t>Spiridinov, V.P.</t>
+    <t>spiridinov, v.p</t>
   </si>
   <si>
     <t>computadoras y procesamiento de datos</t>
   </si>
   <si>
-    <t>Villanueva-Lara, Julio E</t>
-  </si>
-  <si>
-    <t>Introducción a la programación y a las estructuras de datos</t>
-  </si>
-  <si>
-    <t>Braunstein, Silvia L</t>
-  </si>
-  <si>
-    <t>Sheldom M. Ross</t>
+    <t>villanueva-lara, julio e</t>
+  </si>
+  <si>
+    <t>introducción a la programación y a las estructuras de datos</t>
+  </si>
+  <si>
+    <t>braunstein, silvia l</t>
   </si>
   <si>
     <t>introducción a la estadística</t>
   </si>
   <si>
-    <t>Procesamiento de datos y análisis estadísticos</t>
-  </si>
-  <si>
-    <t>Castañeda, Ma. Belén</t>
-  </si>
-  <si>
-    <t>grossman, stanley i.</t>
-  </si>
-  <si>
-    <t>Algebra lineal.</t>
+    <t>sheldom m. ross</t>
+  </si>
+  <si>
+    <t>procesamiento de datos y análisis estadísticos</t>
+  </si>
+  <si>
+    <t>castañeda, ma. belén</t>
+  </si>
+  <si>
+    <t>tratado de derecho administrativo 5</t>
   </si>
 </sst>
 </file>
@@ -783,16 +756,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="76.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,10 +788,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -831,7 +802,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -845,7 +816,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -853,13 +824,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -867,13 +838,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>90</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -881,13 +852,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -895,13 +866,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -909,13 +880,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -923,13 +894,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -937,310 +908,310 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
         <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
         <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
         <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1248,13 +1219,13 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1262,13 +1233,13 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1276,629 +1247,629 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
         <v>17</v>
-      </c>
-      <c r="D35" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D39" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D40" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D45" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D49" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D50" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D51" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C52" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D54" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="D55" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="D56" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D57" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D58" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D59" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="D60" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D61" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D62" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C63" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="D63" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D64" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="D65" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C66" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="D66" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B67" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D67" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D68" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D69" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="D70" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C71" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D71" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B72" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C72" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D72" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B73" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C73" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="D73" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B74" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B75" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C75" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="D75" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C76" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77" t="s">
+        <v>68</v>
+      </c>
+      <c r="C77" t="s">
         <v>8</v>
       </c>
-      <c r="B77" t="s">
-        <v>42</v>
-      </c>
-      <c r="C77" t="s">
-        <v>90</v>
-      </c>
       <c r="D77" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C78" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B79" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,13 +1877,13 @@
         <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C80" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D80" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,13 +1891,13 @@
         <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C81" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="D81" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,13 +1905,13 @@
         <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C82" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="D82" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1948,13 +1919,13 @@
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C83" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="D83" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1962,13 +1933,13 @@
         <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C84" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="D84" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,13 +1947,13 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C85" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="D85" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,13 +1961,13 @@
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C86" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="D86" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2004,13 +1975,13 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C87" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2018,13 +1989,13 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C88" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="D88" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2032,13 +2003,13 @@
         <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C89" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D89" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2046,13 +2017,13 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C90" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="D90" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,13 +2031,13 @@
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C91" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="D91" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,13 +2045,13 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C92" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="D92" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2088,13 +2059,13 @@
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C93" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="D93" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,13 +2073,13 @@
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C94" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="D94" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,13 +2087,13 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C95" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="D95" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2130,13 +2101,13 @@
         <v>4</v>
       </c>
       <c r="B96" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C96" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="D96" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2144,13 +2115,13 @@
         <v>4</v>
       </c>
       <c r="B97" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C97" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="D97" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,13 +2129,13 @@
         <v>4</v>
       </c>
       <c r="B98" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C98" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D98" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2172,13 +2143,13 @@
         <v>4</v>
       </c>
       <c r="B99" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C99" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D99" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,13 +2157,13 @@
         <v>4</v>
       </c>
       <c r="B100" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C100" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D100" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,13 +2171,13 @@
         <v>4</v>
       </c>
       <c r="B101" t="s">
+        <v>108</v>
+      </c>
+      <c r="C101" t="s">
+        <v>115</v>
+      </c>
+      <c r="D101" t="s">
         <v>116</v>
-      </c>
-      <c r="C101" t="s">
-        <v>123</v>
-      </c>
-      <c r="D101" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2214,13 +2185,13 @@
         <v>4</v>
       </c>
       <c r="B102" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C102" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D102" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2228,13 +2199,13 @@
         <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C103" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D103" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2242,17 +2213,16 @@
         <v>4</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C104" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D104" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>